<commit_message>
BUG: Don't extract header names if none specified
Closes gh-11733.
</commit_message>
<xml_diff>
--- a/pandas/tests/io/data/testmultiindex.xlsx
+++ b/pandas/tests/io/data/testmultiindex.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anaconda3\Lib\site-packages\pandas\io\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beano\Repositories\pandas\pandas\tests\io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62484658-60B6-4AFE-9718-E1BB2EECC154}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="single_column_name" sheetId="9" r:id="rId1"/>
@@ -21,6 +22,7 @@
     <sheet name="mi_index_name" sheetId="7" r:id="rId7"/>
     <sheet name="both_name" sheetId="8" r:id="rId8"/>
     <sheet name="both_name_skiprows" sheetId="10" r:id="rId9"/>
+    <sheet name="index_col_none" sheetId="13" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -61,11 +63,23 @@
   <si>
     <t>ilvl2</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
@@ -121,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -157,6 +171,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,7 +203,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -278,6 +295,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -313,6 +347,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -488,16 +539,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -514,7 +565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -531,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -548,7 +599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -565,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -587,17 +638,89 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC70534C-1941-4D3C-AD60-169D2BD8790A}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13">
+        <v>3</v>
+      </c>
+      <c r="D3" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13">
+        <v>3</v>
+      </c>
+      <c r="D4" s="13">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="12" t="s">
         <v>4</v>
@@ -608,7 +731,7 @@
       </c>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -623,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -640,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -657,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -674,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -701,14 +824,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
@@ -724,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -744,7 +867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>1</v>
@@ -762,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -782,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
         <v>1</v>
@@ -806,16 +929,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="5"/>
       <c r="C1" s="12" t="s">
         <v>4</v>
@@ -826,7 +949,7 @@
       </c>
       <c r="F1" s="12"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -841,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
@@ -861,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="5" t="s">
         <v>1</v>
@@ -879,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
@@ -899,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="5" t="s">
         <v>1</v>
@@ -929,16 +1052,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -951,7 +1074,7 @@
       </c>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -968,7 +1091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -985,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1002,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1019,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1046,16 +1169,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -1068,7 +1191,7 @@
       </c>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -1085,7 +1208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>0</v>
       </c>
@@ -1102,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -1119,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -1136,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>3</v>
       </c>
@@ -1163,16 +1286,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -1192,7 +1315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -1212,7 +1335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -1230,7 +1353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
@@ -1250,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -1278,16 +1401,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
@@ -1300,7 +1423,7 @@
       </c>
       <c r="F1" s="12"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1317,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1329,7 +1452,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
@@ -1349,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -1367,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
@@ -1387,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="6" t="s">
         <v>1</v>
@@ -1417,16 +1540,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A3:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1439,7 +1562,7 @@
       </c>
       <c r="F3" s="12"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1456,7 +1579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1468,7 +1591,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
@@ -1488,7 +1611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="9" t="s">
         <v>1</v>
@@ -1506,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
@@ -1526,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="9" t="s">
         <v>1</v>

</xml_diff>